<commit_message>
termine de medir con el puente falta analiza impedancias
</commit_message>
<xml_diff>
--- a/TP4/capacitorescaca.xlsx
+++ b/TP4/capacitorescaca.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OperaDownload\Laboratorio Electronica\lab-electronica\TP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40622AAB-B29E-4515-A8FD-5887DAC968B4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1824A23F-D388-4713-860B-B3C4F270F4A4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" xr2:uid="{8FECFAAB-4C3B-4091-94B8-C098B3764CF4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" activeTab="2" xr2:uid="{8FECFAAB-4C3B-4091-94B8-C098B3764CF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
   <si>
     <t>f</t>
   </si>
@@ -72,6 +74,39 @@
   </si>
   <si>
     <t>150n</t>
+  </si>
+  <si>
+    <t>Rx medido</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>C[nF]</t>
+  </si>
+  <si>
+    <t>R[Omega]</t>
+  </si>
+  <si>
+    <t>Grados</t>
+  </si>
+  <si>
+    <t>31.36n</t>
   </si>
 </sst>
 </file>
@@ -426,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EBEDB5-37D4-4285-945B-B24BD82F646C}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,4 +766,556 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1411D2-1BA8-4893-8A3B-96931330E94B}">
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>82</v>
+      </c>
+      <c r="D2">
+        <v>77</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10440</v>
+      </c>
+      <c r="F2" s="1">
+        <f>$O$3*0.000000001*10000/(E2)</f>
+        <v>6.688697318007663E-9</v>
+      </c>
+      <c r="G2" s="1">
+        <f>2*PI()*D2*A2*$O$3*0.000000001</f>
+        <v>3.3784121910026992E-2</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2" s="1">
+        <f>D2*E2/10000</f>
+        <v>80.388000000000005</v>
+      </c>
+      <c r="K2">
+        <v>83.1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O2">
+        <v>7.0330000000000004</v>
+      </c>
+      <c r="P2" s="1">
+        <v>140</v>
+      </c>
+      <c r="Q2">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="R2">
+        <v>-89.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>57.1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2210</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F5" si="0">$O$3*0.000000001*10000/(E3)</f>
+        <v>3.1597285067873302E-8</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G15" si="1">2*PI()*D3*A3*$O$3*0.000000001</f>
+        <v>2.5052900793020014E-2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>-75</v>
+      </c>
+      <c r="I3" s="1">
+        <f>D3*E3/10000</f>
+        <v>12.6191</v>
+      </c>
+      <c r="K3">
+        <v>19.7</v>
+      </c>
+      <c r="N3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="O3">
+        <v>6.9829999999999997</v>
+      </c>
+      <c r="P3" s="1">
+        <v>66</v>
+      </c>
+      <c r="Q3">
+        <v>2.9100000000000001E-2</v>
+      </c>
+      <c r="R3">
+        <v>-88.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D4">
+        <v>47.3</v>
+      </c>
+      <c r="E4">
+        <v>1025</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>6.8126829268292684E-8</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>2.075310345901658E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1">
+        <f>D4*E4/10000</f>
+        <v>4.8482500000000002</v>
+      </c>
+      <c r="K4">
+        <v>9.4</v>
+      </c>
+      <c r="N4" s="1">
+        <v>100000</v>
+      </c>
+      <c r="O4">
+        <v>6.8470000000000004</v>
+      </c>
+      <c r="P4" s="1">
+        <v>30.8</v>
+      </c>
+      <c r="Q4">
+        <v>0.13320000000000001</v>
+      </c>
+      <c r="R4">
+        <v>-82.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>3.2</v>
+      </c>
+      <c r="D5">
+        <v>62.3</v>
+      </c>
+      <c r="E5">
+        <v>455</v>
+      </c>
+      <c r="F5" s="1">
+        <f>$O$3*0.000000001*10000/(E5)</f>
+        <v>1.5347252747252749E-7</v>
+      </c>
+      <c r="G5" s="1">
+        <f>2*PI()*D5*A5*$O$3*0.000000001</f>
+        <v>2.7334425909021833E-2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1">
+        <f>D5*E5/10000</f>
+        <v>2.8346499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D7">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>1023</v>
+      </c>
+      <c r="F7" s="1">
+        <f>$O$2*0.000000001*10000/(E7)</f>
+        <v>6.874877810361683E-8</v>
+      </c>
+      <c r="G7" s="1">
+        <f>2*PI()*D7*A7*$O$2*0.000000001</f>
+        <v>2.1652924710043073E-3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1">
+        <f>D7*E7/10000</f>
+        <v>5.0126999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>52.3</v>
+      </c>
+      <c r="E8">
+        <v>2190</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" ref="F8:F10" si="2">$O$2*0.000000001*10000/(E8)</f>
+        <v>3.2114155251141555E-8</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G10" si="3">2*PI()*D8*A8*$O$2*0.000000001</f>
+        <v>2.3111182904801079E-3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="1">
+        <f>D8*E8/10000</f>
+        <v>11.4537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>82</v>
+      </c>
+      <c r="D9">
+        <v>77</v>
+      </c>
+      <c r="E9">
+        <v>10450</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="2"/>
+        <v>6.7301435406698576E-9</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="3"/>
+        <v>3.4026024544353403E-3</v>
+      </c>
+      <c r="H9">
+        <v>-140</v>
+      </c>
+      <c r="I9" s="1">
+        <f>D9*E9/10000</f>
+        <v>80.465000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>3.2</v>
+      </c>
+      <c r="D10">
+        <v>63.5</v>
+      </c>
+      <c r="E10">
+        <v>456</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5423245614035091E-7</v>
+      </c>
+      <c r="G10" s="1">
+        <f>2*PI()*D10*A10*$O$2*0.000000001</f>
+        <v>2.8060422838525217E-3</v>
+      </c>
+      <c r="I10" s="1">
+        <f>D10*E10/10000</f>
+        <v>2.8956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D12">
+        <v>46.2</v>
+      </c>
+      <c r="E12">
+        <v>1193</v>
+      </c>
+      <c r="F12" s="1">
+        <f>$O$4*0.000000001*10000/(E12)</f>
+        <v>5.7393126571668072E-8</v>
+      </c>
+      <c r="G12" s="1">
+        <f>2*PI()*D12*A12*$O$4*0.000000001</f>
+        <v>0.19875688046795487</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="1">
+        <f>D12*E12/10000</f>
+        <v>5.5116600000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>50.5</v>
+      </c>
+      <c r="E13">
+        <v>2520</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" ref="F13:F15" si="4">$O$4*0.000000001*10000/(E13)</f>
+        <v>2.7170634920634927E-8</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" ref="G13:G15" si="5">2*PI()*D13*A13*$O$4*0.000000001</f>
+        <v>0.21725589748120611</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" ref="I13:I15" si="6">D13*E13/10000</f>
+        <v>12.726000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>81</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10445</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="4"/>
+        <v>6.5552896122546687E-9</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="5"/>
+        <v>0.34846985536589492</v>
+      </c>
+      <c r="H14">
+        <v>47</v>
+      </c>
+      <c r="I14" s="1">
+        <f>D14*E14/10000</f>
+        <v>84.604500000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>3.2</v>
+      </c>
+      <c r="D15">
+        <v>54</v>
+      </c>
+      <c r="E15">
+        <v>525</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="4"/>
+        <v>1.3041904761904763E-7</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="5"/>
+        <v>0.2323132369105966</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="6"/>
+        <v>2.835</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6ECAE73-945A-4A47-B029-1DB87B48E7ED}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TERMINEEEEEE DE MEDIRRRR....ni idea si esta bien pero ya fue
</commit_message>
<xml_diff>
--- a/TP4/capacitorescaca.xlsx
+++ b/TP4/capacitorescaca.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OperaDownload\Laboratorio Electronica\lab-electronica\TP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1824A23F-D388-4713-860B-B3C4F270F4A4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89836C1F-F3C7-41B5-A9C3-583C621BFDFD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" activeTab="2" xr2:uid="{8FECFAAB-4C3B-4091-94B8-C098B3764CF4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" activeTab="1" xr2:uid="{8FECFAAB-4C3B-4091-94B8-C098B3764CF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
   <si>
     <t>f</t>
   </si>
@@ -106,7 +105,46 @@
     <t>Grados</t>
   </si>
   <si>
-    <t>31.36n</t>
+    <t>Puente</t>
+  </si>
+  <si>
+    <t>Analizador de Impedancia</t>
+  </si>
+  <si>
+    <t>rx</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>.15k</t>
+  </si>
+  <si>
+    <t>.114k</t>
+  </si>
+  <si>
+    <t>.0993k</t>
+  </si>
+  <si>
+    <t>.041k</t>
+  </si>
+  <si>
+    <t>0.0238k</t>
+  </si>
+  <si>
+    <t>.019k</t>
+  </si>
+  <si>
+    <t>.0115k</t>
+  </si>
+  <si>
+    <t>.010k</t>
+  </si>
+  <si>
+    <t>.0066k</t>
+  </si>
+  <si>
+    <t>NO USAR ESTA PAGINA</t>
   </si>
 </sst>
 </file>
@@ -459,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EBEDB5-37D4-4285-945B-B24BD82F646C}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,6 +801,11 @@
         <v>6.9119999999999999</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -770,10 +813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1411D2-1BA8-4893-8A3B-96931330E94B}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,31 +827,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
         <v>14</v>
@@ -830,35 +849,32 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>10000</v>
+      <c r="A2" t="s">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>82</v>
-      </c>
-      <c r="D2">
-        <v>77</v>
-      </c>
-      <c r="E2" s="1">
-        <v>10440</v>
-      </c>
-      <c r="F2" s="1">
-        <f>$O$3*0.000000001*10000/(E2)</f>
-        <v>6.688697318007663E-9</v>
-      </c>
-      <c r="G2" s="1">
-        <f>2*PI()*D2*A2*$O$3*0.000000001</f>
-        <v>3.3784121910026992E-2</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2" s="1">
-        <f>D2*E2/10000</f>
-        <v>80.388000000000005</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
       </c>
       <c r="K2">
         <v>83.1</v>
@@ -884,31 +900,31 @@
         <v>10000</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D3">
-        <v>57.1</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1">
-        <v>2210</v>
+        <v>10440</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F5" si="0">$O$3*0.000000001*10000/(E3)</f>
-        <v>3.1597285067873302E-8</v>
+        <f>$O$3*0.000000001*10000/(E3)</f>
+        <v>6.688697318007663E-9</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G15" si="1">2*PI()*D3*A3*$O$3*0.000000001</f>
-        <v>2.5052900793020014E-2</v>
-      </c>
-      <c r="H3" s="1">
-        <v>-75</v>
+        <f>2*PI()*D3*A3*$O$3*0.000000001</f>
+        <v>3.3784121910026992E-2</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
       </c>
       <c r="I3" s="1">
         <f>D3*E3/10000</f>
-        <v>12.6191</v>
+        <v>80.388000000000005</v>
       </c>
       <c r="K3">
         <v>19.7</v>
@@ -934,31 +950,31 @@
         <v>10000</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>8.1999999999999993</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>47.3</v>
-      </c>
-      <c r="E4">
-        <v>1025</v>
+        <v>57.1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2210</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>6.8126829268292684E-8</v>
+        <f t="shared" ref="F4:F5" si="0">$O$3*0.000000001*10000/(E4)</f>
+        <v>3.1597285067873302E-8</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>2.075310345901658E-2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
+        <f t="shared" ref="G4:G5" si="1">2*PI()*D4*A4*$O$3*0.000000001</f>
+        <v>2.5052900793020014E-2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-75</v>
       </c>
       <c r="I4" s="1">
         <f>D4*E4/10000</f>
-        <v>4.8482500000000002</v>
+        <v>12.6191</v>
       </c>
       <c r="K4">
         <v>9.4</v>
@@ -984,101 +1000,101 @@
         <v>10000</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>3.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D5">
-        <v>62.3</v>
+        <v>47.3</v>
       </c>
       <c r="E5">
-        <v>455</v>
+        <v>1025</v>
       </c>
       <c r="F5" s="1">
-        <f>$O$3*0.000000001*10000/(E5)</f>
-        <v>1.5347252747252749E-7</v>
+        <f t="shared" si="0"/>
+        <v>6.8126829268292684E-8</v>
       </c>
       <c r="G5" s="1">
-        <f>2*PI()*D5*A5*$O$3*0.000000001</f>
-        <v>2.7334425909021833E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.075310345901658E-2</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="1">
         <f>D5*E5/10000</f>
+        <v>4.8482500000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>3.2</v>
+      </c>
+      <c r="D6">
+        <v>62.3</v>
+      </c>
+      <c r="E6">
+        <v>455</v>
+      </c>
+      <c r="F6" s="1">
+        <f>$O$3*0.000000001*10000/(E6)</f>
+        <v>1.5347252747252749E-7</v>
+      </c>
+      <c r="G6" s="1">
+        <f>2*PI()*D6*A6*$O$3*0.000000001</f>
+        <v>2.7334425909021833E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1">
+        <f>D6*E6/10000</f>
         <v>2.8346499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D7">
-        <v>49</v>
-      </c>
-      <c r="E7">
-        <v>1023</v>
-      </c>
-      <c r="F7" s="1">
-        <f>$O$2*0.000000001*10000/(E7)</f>
-        <v>6.874877810361683E-8</v>
-      </c>
-      <c r="G7" s="1">
-        <f>2*PI()*D7*A7*$O$2*0.000000001</f>
-        <v>2.1652924710043073E-3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="1">
-        <f>D7*E7/10000</f>
-        <v>5.0126999999999997</v>
-      </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1000</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>18</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D8">
-        <v>52.3</v>
+        <v>49</v>
       </c>
       <c r="E8">
-        <v>2190</v>
+        <v>1023</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F10" si="2">$O$2*0.000000001*10000/(E8)</f>
-        <v>3.2114155251141555E-8</v>
+        <f>$O$2*0.000000001*10000/(E8)</f>
+        <v>6.874877810361683E-8</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G10" si="3">2*PI()*D8*A8*$O$2*0.000000001</f>
-        <v>2.3111182904801079E-3</v>
+        <f>2*PI()*D8*A8*$O$2*0.000000001</f>
+        <v>2.1652924710043073E-3</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="1">
         <f>D8*E8/10000</f>
-        <v>11.4537</v>
+        <v>5.0126999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1086,31 +1102,31 @@
         <v>1000</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>77</v>
+        <v>52.3</v>
       </c>
       <c r="E9">
-        <v>10450</v>
+        <v>2190</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="2"/>
-        <v>6.7301435406698576E-9</v>
+        <f t="shared" ref="F9:F11" si="2">$O$2*0.000000001*10000/(E9)</f>
+        <v>3.2114155251141555E-8</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="3"/>
-        <v>3.4026024544353403E-3</v>
-      </c>
-      <c r="H9">
-        <v>-140</v>
+        <f t="shared" ref="G9:G10" si="3">2*PI()*D9*A9*$O$2*0.000000001</f>
+        <v>2.3111182904801079E-3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
       </c>
       <c r="I9" s="1">
         <f>D9*E9/10000</f>
-        <v>80.465000000000003</v>
+        <v>11.4537</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1118,98 +1134,98 @@
         <v>1000</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>3.2</v>
+        <v>82</v>
       </c>
       <c r="D10">
-        <v>63.5</v>
+        <v>77</v>
       </c>
       <c r="E10">
-        <v>456</v>
+        <v>10450</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="2"/>
-        <v>1.5423245614035091E-7</v>
+        <v>6.7301435406698576E-9</v>
       </c>
       <c r="G10" s="1">
-        <f>2*PI()*D10*A10*$O$2*0.000000001</f>
-        <v>2.8060422838525217E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.4026024544353403E-3</v>
+      </c>
+      <c r="H10">
+        <v>-140</v>
       </c>
       <c r="I10" s="1">
         <f>D10*E10/10000</f>
+        <v>80.465000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>3.2</v>
+      </c>
+      <c r="D11">
+        <v>63.5</v>
+      </c>
+      <c r="E11">
+        <v>456</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5423245614035091E-7</v>
+      </c>
+      <c r="G11" s="1">
+        <f>2*PI()*D11*A11*$O$2*0.000000001</f>
+        <v>2.8060422838525217E-3</v>
+      </c>
+      <c r="I11" s="1">
+        <f>D11*E11/10000</f>
         <v>2.8956</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>100000</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="D12">
-        <v>46.2</v>
-      </c>
-      <c r="E12">
-        <v>1193</v>
-      </c>
-      <c r="F12" s="1">
-        <f>$O$4*0.000000001*10000/(E12)</f>
-        <v>5.7393126571668072E-8</v>
-      </c>
-      <c r="G12" s="1">
-        <f>2*PI()*D12*A12*$O$4*0.000000001</f>
-        <v>0.19875688046795487</v>
-      </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="1">
-        <f>D12*E12/10000</f>
-        <v>5.5116600000000009</v>
-      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>100000</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>18</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D13">
-        <v>50.5</v>
+        <v>46.2</v>
       </c>
       <c r="E13">
-        <v>2520</v>
+        <v>1193</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" ref="F13:F15" si="4">$O$4*0.000000001*10000/(E13)</f>
-        <v>2.7170634920634927E-8</v>
+        <f>$O$4*0.000000001*10000/(E13)</f>
+        <v>5.7393126571668072E-8</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ref="G13:G15" si="5">2*PI()*D13*A13*$O$4*0.000000001</f>
-        <v>0.21725589748120611</v>
+        <f>2*PI()*D13*A13*$O$4*0.000000001</f>
+        <v>0.19875688046795487</v>
       </c>
       <c r="H13" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" ref="I13:I15" si="6">D13*E13/10000</f>
-        <v>12.726000000000001</v>
+        <f>D13*E13/10000</f>
+        <v>5.5116600000000009</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1217,31 +1233,31 @@
         <v>100000</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="D14">
-        <v>81</v>
-      </c>
-      <c r="E14" s="1">
-        <v>10445</v>
+        <v>50.5</v>
+      </c>
+      <c r="E14">
+        <v>2520</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="4"/>
-        <v>6.5552896122546687E-9</v>
+        <f t="shared" ref="F14:F16" si="4">$O$4*0.000000001*10000/(E14)</f>
+        <v>2.7170634920634927E-8</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="5"/>
-        <v>0.34846985536589492</v>
-      </c>
-      <c r="H14">
-        <v>47</v>
+        <f t="shared" ref="G14:G16" si="5">2*PI()*D14*A14*$O$4*0.000000001</f>
+        <v>0.21725589748120611</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
       </c>
       <c r="I14" s="1">
-        <f>D14*E14/10000</f>
-        <v>84.604500000000002</v>
+        <f t="shared" ref="I14:I16" si="6">D14*E14/10000</f>
+        <v>12.726000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -1249,70 +1265,346 @@
         <v>100000</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>3.2</v>
+        <v>82</v>
       </c>
       <c r="D15">
-        <v>54</v>
-      </c>
-      <c r="E15">
-        <v>525</v>
+        <v>81</v>
+      </c>
+      <c r="E15" s="1">
+        <v>10445</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="4"/>
-        <v>1.3041904761904763E-7</v>
+        <v>6.5552896122546687E-9</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="5"/>
+        <v>0.34846985536589492</v>
+      </c>
+      <c r="H15">
+        <v>47</v>
+      </c>
+      <c r="I15" s="1">
+        <f>D15*E15/10000</f>
+        <v>84.604500000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>3.2</v>
+      </c>
+      <c r="D16">
+        <v>54</v>
+      </c>
+      <c r="E16">
+        <v>525</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="4"/>
+        <v>1.3041904761904763E-7</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="5"/>
         <v>0.2323132369105966</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I16" s="1">
         <f t="shared" si="6"/>
         <v>2.835</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6ECAE73-945A-4A47-B029-1DB87B48E7ED}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>82</v>
+      </c>
+      <c r="D20">
+        <v>6.4630000000000001</v>
+      </c>
+      <c r="E20">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="F20">
+        <v>-89.66</v>
+      </c>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C21">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D21">
+        <v>31.46</v>
+      </c>
+      <c r="E21">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="F21">
+        <v>-89.69</v>
+      </c>
+      <c r="G21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D22">
+        <v>67.45</v>
+      </c>
+      <c r="E22">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="F22">
+        <v>-89.55</v>
+      </c>
+      <c r="G22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>3.2</v>
+      </c>
+      <c r="D23">
+        <v>152.35</v>
+      </c>
+      <c r="E23">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="F23">
+        <v>-89.5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>82</v>
+      </c>
+      <c r="D25">
+        <v>6.43</v>
+      </c>
+      <c r="E25">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="F25">
+        <v>-87.12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>31.19</v>
+      </c>
+      <c r="E26">
+        <v>4.65E-2</v>
+      </c>
+      <c r="F26">
+        <v>-87.3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D27">
+        <v>66.849999999999994</v>
+      </c>
+      <c r="E27">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="F27">
+        <v>-87.2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>3.2</v>
+      </c>
+      <c r="D28">
+        <v>151</v>
+      </c>
+      <c r="E28">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="F28">
+        <v>-86.4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>82</v>
+      </c>
+      <c r="D30">
+        <v>6.3360000000000003</v>
+      </c>
+      <c r="E30">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="F30">
+        <v>-68.44</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>30.95</v>
+      </c>
+      <c r="E31">
+        <v>0.39369999999999999</v>
+      </c>
+      <c r="F31">
+        <v>-68.510000000000005</v>
+      </c>
+      <c r="G31">
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D32">
+        <v>67.290000000000006</v>
+      </c>
+      <c r="E32">
+        <v>0.42080000000000001</v>
+      </c>
+      <c r="F32">
+        <v>-67.19</v>
+      </c>
+      <c r="G32">
+        <v>9.9600000000000009</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>3.2</v>
+      </c>
+      <c r="D33">
+        <v>156.69999999999999</v>
+      </c>
+      <c r="E33">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F33">
+        <v>-60.12</v>
+      </c>
+      <c r="G33">
+        <v>5.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error relativo maso esta
</commit_message>
<xml_diff>
--- a/TP4/capacitorescaca.xlsx
+++ b/TP4/capacitorescaca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OperaDownload\Laboratorio Electronica\lab-electronica\TP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB452AE8-B9F5-417E-BFBA-146E622CE1B0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC725CB8-7F4C-43CF-B666-897F904FEA68}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" activeTab="1" xr2:uid="{8FECFAAB-4C3B-4091-94B8-C098B3764CF4}"/>
   </bookViews>
@@ -141,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,13 +149,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1411D2-1BA8-4893-8A3B-96931330E94B}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30:P33"/>
+    <sheetView tabSelected="1" topLeftCell="H18" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,16 +1349,17 @@
       <c r="K19" t="s">
         <v>24</v>
       </c>
-      <c r="M19" t="s">
+      <c r="L19" s="3"/>
+      <c r="M19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1369,22 +1388,22 @@
       <c r="K20" s="1">
         <v>1000</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="4">
         <f>ABS((D20*0.000000001-F8)/(D20*0.000000001))*100</f>
         <v>4.1334293775314421</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="4">
         <f>ABS((E20-G8)/E20)*100</f>
         <v>46.834336649447813</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="4">
         <f>ABS((F20-H8)/F20)*100</f>
         <v>0.16729868391702618</v>
       </c>
-      <c r="P20" s="1">
+      <c r="P20" s="4">
         <f>ABS((G20-I8)/G20)*100</f>
         <v>46.356666666666662</v>
       </c>
@@ -1414,22 +1433,22 @@
       <c r="K21" s="1">
         <v>1000</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="4">
         <f t="shared" ref="M21:M23" si="7">ABS((D21*0.000000001-F9)/(D21*0.000000001))*100</f>
         <v>2.0793237480659568</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="4">
         <f t="shared" ref="N21:N23" si="8">ABS((E21-G9)/E21)*100</f>
         <v>69.185089460265232</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="4">
         <f t="shared" ref="O21:O23" si="9">ABS((F21-H9)/F21)*100</f>
         <v>0.20069126992976566</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" s="4">
         <f t="shared" ref="P21:P23" si="10">ABS((G21-I9)/G21)*100</f>
         <v>72.064146341463413</v>
       </c>
@@ -1459,22 +1478,22 @@
       <c r="K22" s="1">
         <v>1000</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="4">
         <f t="shared" si="7"/>
         <v>1.9255420364963947</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="4">
         <f t="shared" si="8"/>
         <v>72.239840115329386</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="4">
         <f t="shared" si="9"/>
         <v>0.36850921273031639</v>
       </c>
-      <c r="P22" s="1">
+      <c r="P22" s="4">
         <f t="shared" si="10"/>
         <v>73.617368421052646</v>
       </c>
@@ -1504,25 +1523,31 @@
       <c r="K23" s="1">
         <v>1000</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="4">
         <f t="shared" si="7"/>
         <v>1.2356128259605517</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="4">
         <f t="shared" si="8"/>
         <v>70.462712801552414</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="4">
         <f t="shared" si="9"/>
         <v>0.3798882681564284</v>
       </c>
-      <c r="P23" s="1">
+      <c r="P23" s="4">
         <f t="shared" si="10"/>
         <v>71.043999999999997</v>
       </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -1552,19 +1577,19 @@
       <c r="L25" t="s">
         <v>8</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="2">
         <f>ABS((D25*0.000000001-F3)/(D25*0.000000001))*100</f>
         <v>4.0232864386883778</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="2">
         <f>ABS((E25-G3)/E25)*100</f>
         <v>26.715570694084622</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="2">
         <f>ABS((F25-H3)/F25)*100</f>
         <v>1.1248852157942948</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P25" s="2">
         <f>ABS((G25-I3)/G25)*100</f>
         <v>29.484210526315785</v>
       </c>
@@ -1591,19 +1616,19 @@
       <c r="L26" t="s">
         <v>10</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="2">
         <f t="shared" ref="M26:M28" si="11">ABS((D26*0.000000001-F4)/(D26*0.000000001))*100</f>
         <v>1.3058193904241713</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="2">
         <f t="shared" ref="N26:N28" si="12">ABS((E26-G4)/E26)*100</f>
         <v>46.122793993505347</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="2">
         <f t="shared" ref="O26:O28" si="13">ABS((F26-H4)/F26)*100</f>
         <v>1.4432989690721709</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P26" s="2">
         <f t="shared" ref="P26:P28" si="14">ABS((G26-I4)/G26)*100</f>
         <v>46.978571428571428</v>
       </c>
@@ -1630,19 +1655,19 @@
       <c r="L27" t="s">
         <v>12</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="2">
         <f t="shared" si="11"/>
         <v>1.9099914260174877</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="2">
         <f t="shared" si="12"/>
         <v>57.210095960790554</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="2">
         <f t="shared" si="13"/>
         <v>1.8463302752293571</v>
       </c>
-      <c r="P27" s="1">
+      <c r="P27" s="2">
         <f t="shared" si="14"/>
         <v>57.841304347826082</v>
       </c>
@@ -1669,22 +1694,28 @@
       <c r="L28" t="s">
         <v>13</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="2">
         <f t="shared" si="11"/>
         <v>1.637435412269848</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="2">
         <f t="shared" si="12"/>
         <v>55.840992069431607</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="2">
         <f t="shared" si="13"/>
         <v>2.3495370370370381</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P28" s="2">
         <f t="shared" si="14"/>
         <v>57.050757575757572</v>
       </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -1714,19 +1745,19 @@
       <c r="L30" t="s">
         <v>8</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="2">
         <f>ABS((D30*0.000000001-F13)/(D30*0.000000001))*100</f>
         <v>3.4610102944234251</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="2">
         <f>ABS((E30-G13)/E30)*100</f>
         <v>11.779783451672177</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="2">
         <f>ABS((F30-H13)/F30)*100</f>
         <v>3.4482758620689649</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30" s="2">
         <f>ABS((G30-I13)/G30)*100</f>
         <v>14.799093655589122</v>
       </c>
@@ -1753,19 +1784,19 @@
       <c r="L31" t="s">
         <v>10</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="2">
         <f t="shared" ref="M31:M33" si="15">ABS((D31*0.000000001-F14)/(D31*0.000000001))*100</f>
         <v>12.21119573300509</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="2">
         <f t="shared" ref="N31:N33" si="16">ABS((E31-G14)/E31)*100</f>
         <v>44.816891673556995</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="2">
         <f t="shared" ref="O31:O33" si="17">ABS((F31-H14)/F31)*100</f>
         <v>13.530871405634207</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P31" s="2">
         <f t="shared" ref="P31:P33" si="18">ABS((G31-I14)/G31)*100</f>
         <v>37.155555555555551</v>
       </c>
@@ -1792,19 +1823,19 @@
       <c r="L32" t="s">
         <v>12</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="2">
         <f t="shared" si="15"/>
         <v>14.707792284636561</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="2">
         <f t="shared" si="16"/>
         <v>52.766901029478404</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="2">
         <f t="shared" si="17"/>
         <v>17.219824378627784</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P32" s="2">
         <f t="shared" si="18"/>
         <v>44.662048192771081</v>
       </c>
@@ -1831,19 +1862,19 @@
       <c r="L33" t="s">
         <v>13</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="2">
         <f t="shared" si="15"/>
         <v>16.771507581973427</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="2">
         <f t="shared" si="16"/>
         <v>59.314669542802697</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="2">
         <f t="shared" si="17"/>
         <v>27.944111776447112</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P33" s="2">
         <f t="shared" si="18"/>
         <v>51.372212692967409</v>
       </c>

</xml_diff>